<commit_message>
Journal de travail du 13 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16896E76-A936-4890-9526-6B5BF5A08E24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80954E9-0AE5-4884-8CD3-0C199A08D7C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -103,13 +103,39 @@
     <t>Planification initiale.</t>
   </si>
   <si>
-    <t>Page de garde                                                                                                                                                                                                                                              Introduction                                                                                                                                                                                                                        Objectifs                                                                                                                                                                                                                                        Planification initiale</t>
-  </si>
-  <si>
     <t>Mise en place du repository Github.</t>
   </si>
   <si>
     <t>https://github.com/dylanramos/MessagingApp</t>
+  </si>
+  <si>
+    <t>13 mai 2020</t>
+  </si>
+  <si>
+    <t>http://pencil.evolus.vn/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X16IyNbcAr0
+https://csharp-tutorials1.blogspot.com/2016/12/client-server-programming-in-c-chat.html
+https://www.codeproject.com/Articles/429144/Simple-Instant-Messenger-with-SSL-Encryption-in-Cs</t>
+  </si>
+  <si>
+    <t>J'ai cherché quelques informations sur comment utiliser une connexion client / serveur.</t>
+  </si>
+  <si>
+    <t>J'ai utilisé le logiciel Pencil.</t>
+  </si>
+  <si>
+    <t>Page de garde.                                                                                                                                                                                                                                              Introduction.                                                                                                                                                                                                                       Objectifs.                                                                                                                                                                                                                                        Planification initiale.</t>
+  </si>
+  <si>
+    <t>J'ai ajouté les maquettes graphiques au rapport de projet.</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>J'ai ajouté quelques tâches au Sprint 1.</t>
   </si>
 </sst>
 </file>
@@ -330,10 +356,10 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -388,19 +414,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -719,7 +745,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +753,7 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -853,7 +879,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -868,7 +894,7 @@
         <v>0.65625</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D8" ca="1" si="0">IF(ISBLANK(C6), NOW(),C6)-IF(ISBLANK(B6),NOW(),B6)</f>
+        <f t="shared" ref="D6:D10" ca="1" si="0">IF(ISBLANK(C6), NOW(),C6)-IF(ISBLANK(B6),NOW(),B6)</f>
         <v>3.125E-2</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -877,57 +903,169 @@
       <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="21" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="G7" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="D8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="6"/>
+      <c r="G9" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="10">
-        <f ca="1">SUM(D2:D8)</f>
-        <v>0.20833333333333331</v>
+        <f ca="1">SUM(D2:D10)</f>
+        <v>0.41666666666666663</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{B61C7B33-089B-4F0F-A77D-9C8EF418A1B6}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{7C1841B8-440B-4FBE-9A1D-B24C5FAD72AB}"/>
+    <hyperlink ref="H8" r:id="rId3" display="https://www.youtube.com/watch?v=X16IyNbcAr0" xr:uid="{5AD5803C-9AD0-4073-89D8-B5F7AC3429A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -937,13 +1075,13 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E8</xm:sqref>
+          <xm:sqref>E2:E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F0617C8B-663B-4AD5-88B4-0512009C0BDD}">
           <x14:formula1>
-            <xm:f>Données!$B$2:$B$5</xm:f>
+            <xm:f>Données!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F8</xm:sqref>
+          <xm:sqref>F2:F14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -956,7 +1094,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +1124,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +1132,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,12 +1140,15 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail du 14 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80954E9-0AE5-4884-8CD3-0C199A08D7C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D7E3C-4AB5-4381-9B4B-5CDB18240989}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>J'ai ajouté quelques tâches au Sprint 1.</t>
+  </si>
+  <si>
+    <t>14 mai 2020</t>
+  </si>
+  <si>
+    <t>J'ai rédigé tous les cas d'utilisation.</t>
+  </si>
+  <si>
+    <t>J'ai créé le MCD et le MLD de la base de données.</t>
+  </si>
+  <si>
+    <t>J'ai rédigé la stratégie de tests et le dossier de conception.</t>
+  </si>
+  <si>
+    <t>https://material.io/resources/icons/?icon=verified_user&amp;style=baseline</t>
+  </si>
+  <si>
+    <t>J'ai commencé à faire la partie graphique du login et j'y ai mis des icônes</t>
   </si>
 </sst>
 </file>
@@ -370,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,6 +444,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -745,7 +766,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +915,7 @@
         <v>0.65625</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D10" ca="1" si="0">IF(ISBLANK(C6), NOW(),C6)-IF(ISBLANK(B6),NOW(),B6)</f>
+        <f t="shared" ref="D6:D14" ca="1" si="0">IF(ISBLANK(C6), NOW(),C6)-IF(ISBLANK(B6),NOW(),B6)</f>
         <v>3.125E-2</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1015,49 +1036,111 @@
       <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="20"/>
+      <c r="A11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="20"/>
+      <c r="A12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="20"/>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="10">
-        <f ca="1">SUM(D2:D10)</f>
-        <v>0.41666666666666663</v>
+        <f ca="1">SUM(D2:D14)</f>
+        <v>0.62499999999999989</v>
       </c>
     </row>
   </sheetData>
@@ -1066,6 +1149,7 @@
     <hyperlink ref="H6" r:id="rId1" xr:uid="{B61C7B33-089B-4F0F-A77D-9C8EF418A1B6}"/>
     <hyperlink ref="H7" r:id="rId2" xr:uid="{7C1841B8-440B-4FBE-9A1D-B24C5FAD72AB}"/>
     <hyperlink ref="H8" r:id="rId3" display="https://www.youtube.com/watch?v=X16IyNbcAr0" xr:uid="{5AD5803C-9AD0-4073-89D8-B5F7AC3429A2}"/>
+    <hyperlink ref="H14" r:id="rId4" xr:uid="{68FFA688-4DCB-47C3-9B87-9096AD11EE7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Journal de travail du 15 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D7E3C-4AB5-4381-9B4B-5CDB18240989}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298E3232-3A09-4451-B1E1-027BE33F4151}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -153,7 +153,40 @@
     <t>https://material.io/resources/icons/?icon=verified_user&amp;style=baseline</t>
   </si>
   <si>
-    <t>J'ai commencé à faire la partie graphique du login et j'y ai mis des icônes</t>
+    <t>15 mai 2020</t>
+  </si>
+  <si>
+    <t>https://www.codeproject.com/Articles/12893/TCP-IP-Chat-Application-Using-C</t>
+  </si>
+  <si>
+    <t>J'ai terminé la partie graphique du login et de la page de création de compte.</t>
+  </si>
+  <si>
+    <t>J'ai commencé à faire la partie graphique du login et j'y ai mis des icônes.</t>
+  </si>
+  <si>
+    <t>Réunion</t>
+  </si>
+  <si>
+    <t>Réunion avec le chef de projet</t>
+  </si>
+  <si>
+    <t>Nous avons fait un point sur l'avancement du projet.</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>J'ai créé le scipt de la création de la base de données en reprenant des éléments de mon précédent projet.</t>
+  </si>
+  <si>
+    <t>https://github.com/dylanramos/Pre-TPI/blob/master/TicketShare/TicketShare/Classes/DataBaseConnection.cs</t>
+  </si>
+  <si>
+    <t>Communication entre le client et le serveur</t>
+  </si>
+  <si>
+    <t>J'ai recherché des informations sur comment communiquer de client à serveur.</t>
   </si>
 </sst>
 </file>
@@ -766,14 +799,14 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="50.7109375" customWidth="1"/>
   </cols>
@@ -1131,16 +1164,120 @@
         <v>12</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" ref="D15:D18" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D21" s="10">
-        <f ca="1">SUM(D2:D14)</f>
-        <v>0.62499999999999989</v>
+        <f ca="1">SUM(D2:D18)</f>
+        <v>0.83333333333333315</v>
       </c>
     </row>
   </sheetData>
@@ -1150,22 +1287,30 @@
     <hyperlink ref="H7" r:id="rId2" xr:uid="{7C1841B8-440B-4FBE-9A1D-B24C5FAD72AB}"/>
     <hyperlink ref="H8" r:id="rId3" display="https://www.youtube.com/watch?v=X16IyNbcAr0" xr:uid="{5AD5803C-9AD0-4073-89D8-B5F7AC3429A2}"/>
     <hyperlink ref="H14" r:id="rId4" xr:uid="{68FFA688-4DCB-47C3-9B87-9096AD11EE7D}"/>
+    <hyperlink ref="H18" r:id="rId5" xr:uid="{36CFA9FF-3DF6-4952-B42C-E0C4D925832C}"/>
+    <hyperlink ref="H17" r:id="rId6" xr:uid="{93D2EFAA-93F5-4D22-A042-08ECA2BE374D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0130828A-ACDD-452C-A113-199680C5AA6C}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F0617C8B-663B-4AD5-88B4-0512009C0BDD}">
           <x14:formula1>
-            <xm:f>Données!$A$2:$A$6</xm:f>
+            <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E14</xm:sqref>
+          <xm:sqref>F2:F15 F17:F18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F0617C8B-663B-4AD5-88B4-0512009C0BDD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
             <xm:f>Données!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F14</xm:sqref>
+          <xm:sqref>F16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0130828A-ACDD-452C-A113-199680C5AA6C}">
+          <x14:formula1>
+            <xm:f>Données!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1175,15 +1320,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1213,7 +1358,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1221,7 +1366,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1229,10 +1374,28 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail du 19 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298E3232-3A09-4451-B1E1-027BE33F4151}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9163B0A-B57D-41FF-B024-47A844687EFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -187,6 +187,20 @@
   </si>
   <si>
     <t>J'ai recherché des informations sur comment communiquer de client à serveur.</t>
+  </si>
+  <si>
+    <t>19 mai 2020</t>
+  </si>
+  <si>
+    <t>Le client et le serveur peuvent maintenant communiquer de manière asynchrone.</t>
+  </si>
+  <si>
+    <t>J'ai regardé quelques exemples de communication TCP/IP en utilisant les sockets puis j'ai adapté mon code.
+J'ai appris à quoi servent les méthodes "delegate"</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Bq1JhTHlxek
+https://stackoverflow.com/questions/661561/how-do-i-update-the-gui-from-another-thread</t>
   </si>
 </sst>
 </file>
@@ -421,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,7 +464,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -481,6 +494,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -796,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,13 +869,13 @@
       <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -879,13 +894,13 @@
       <c r="E3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -907,7 +922,7 @@
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="6"/>
@@ -932,7 +947,7 @@
       <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="9"/>
@@ -957,10 +972,10 @@
       <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>24</v>
       </c>
     </row>
@@ -984,10 +999,10 @@
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1011,10 +1026,10 @@
       <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1038,10 +1053,10 @@
       <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1063,10 +1078,10 @@
       <c r="F10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1088,10 +1103,10 @@
       <c r="F11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="21"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1113,10 +1128,10 @@
       <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1138,10 +1153,10 @@
       <c r="F13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -1163,10 +1178,10 @@
       <c r="F14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1181,7 +1196,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D18" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D20" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1190,10 +1205,10 @@
       <c r="F15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1215,10 +1230,10 @@
       <c r="F16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1240,10 +1255,10 @@
       <c r="F17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1267,18 +1282,180 @@
       <c r="F18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="21"/>
+    </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="10">
-        <f ca="1">SUM(D2:D18)</f>
-        <v>0.83333333333333315</v>
-      </c>
+      <c r="A21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="21"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="21"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="23"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1287,8 +1464,9 @@
     <hyperlink ref="H7" r:id="rId2" xr:uid="{7C1841B8-440B-4FBE-9A1D-B24C5FAD72AB}"/>
     <hyperlink ref="H8" r:id="rId3" display="https://www.youtube.com/watch?v=X16IyNbcAr0" xr:uid="{5AD5803C-9AD0-4073-89D8-B5F7AC3429A2}"/>
     <hyperlink ref="H14" r:id="rId4" xr:uid="{68FFA688-4DCB-47C3-9B87-9096AD11EE7D}"/>
-    <hyperlink ref="H18" r:id="rId5" xr:uid="{36CFA9FF-3DF6-4952-B42C-E0C4D925832C}"/>
-    <hyperlink ref="H17" r:id="rId6" xr:uid="{93D2EFAA-93F5-4D22-A042-08ECA2BE374D}"/>
+    <hyperlink ref="H17" r:id="rId5" xr:uid="{93D2EFAA-93F5-4D22-A042-08ECA2BE374D}"/>
+    <hyperlink ref="H18" r:id="rId6" xr:uid="{36CFA9FF-3DF6-4952-B42C-E0C4D925832C}"/>
+    <hyperlink ref="H19" r:id="rId7" display="https://www.youtube.com/watch?v=Bq1JhTHlxek" xr:uid="{A1B3EF7B-1A3A-49EE-B18E-02CF810F91E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1298,7 +1476,7 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F18</xm:sqref>
+          <xm:sqref>F2:F15 F17:F31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
@@ -1310,7 +1488,7 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E18</xm:sqref>
+          <xm:sqref>E2:E31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Journal de travail du 20 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9163B0A-B57D-41FF-B024-47A844687EFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2E5714-D9E1-48EC-A3DE-042AD1BA135B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,22 @@
   <si>
     <t>https://www.youtube.com/watch?v=Bq1JhTHlxek
 https://stackoverflow.com/questions/661561/how-do-i-update-the-gui-from-another-thread</t>
+  </si>
+  <si>
+    <t>20 mai 2020</t>
+  </si>
+  <si>
+    <t>J'ai eu des problèmes de communication entre le serveur et le client. J'ai dû regarder plusieurs vidéos sur le sujet.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cHq2lYLA4XY
+https://www.youtube.com/watch?v=p8Nlxtj0sV4</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/4181198/how-to-hash-a-password/10402129#10402129</t>
+  </si>
+  <si>
+    <t>J'ai créé le système de hashage de mot de passe.</t>
   </si>
 </sst>
 </file>
@@ -265,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -430,12 +446,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -496,6 +525,12 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -813,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1231,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D20" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D22" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1341,25 +1376,59 @@
       </c>
       <c r="H20" s="21"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="21"/>
+    <row r="21" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
@@ -1467,6 +1536,7 @@
     <hyperlink ref="H17" r:id="rId5" xr:uid="{93D2EFAA-93F5-4D22-A042-08ECA2BE374D}"/>
     <hyperlink ref="H18" r:id="rId6" xr:uid="{36CFA9FF-3DF6-4952-B42C-E0C4D925832C}"/>
     <hyperlink ref="H19" r:id="rId7" display="https://www.youtube.com/watch?v=Bq1JhTHlxek" xr:uid="{A1B3EF7B-1A3A-49EE-B18E-02CF810F91E8}"/>
+    <hyperlink ref="H22" r:id="rId8" location="10402129" display="https://stackoverflow.com/questions/4181198/how-to-hash-a-password/10402129 - 10402129" xr:uid="{97C9D8AD-91DA-4ABA-B1F9-09B7B6B3C10F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Journal de travail du 21 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2E5714-D9E1-48EC-A3DE-042AD1BA135B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9781AB7C-93AD-43A8-845C-8FBA4C4F64F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -217,6 +217,24 @@
   </si>
   <si>
     <t>J'ai créé le système de hashage de mot de passe.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/15354946/what-is-the-proper-way-of-closing-and-cleaning-up-a-socket-connection</t>
+  </si>
+  <si>
+    <t>Création d'un compte</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>21 mai 2020</t>
+  </si>
+  <si>
+    <t>Le système de communication entre le client est le serveur est terminé.</t>
+  </si>
+  <si>
+    <t>Les systèmes de création d'un compte et de login sont terminés. Mais pour l'instant, le mot de passe est stocké en clair car le hashage ne fonctionne pas.</t>
   </si>
 </sst>
 </file>
@@ -281,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -459,12 +477,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,6 +561,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -849,7 +886,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1268,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D22" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D25" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1430,34 +1467,79 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="19"/>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>65</v>
+      </c>
       <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="19"/>
+      <c r="A25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="27"/>
       <c r="H25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1527,6 +1609,9 @@
       <c r="D35" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G24:G25"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{B61C7B33-089B-4F0F-A77D-9C8EF418A1B6}"/>
@@ -1537,6 +1622,7 @@
     <hyperlink ref="H18" r:id="rId6" xr:uid="{36CFA9FF-3DF6-4952-B42C-E0C4D925832C}"/>
     <hyperlink ref="H19" r:id="rId7" display="https://www.youtube.com/watch?v=Bq1JhTHlxek" xr:uid="{A1B3EF7B-1A3A-49EE-B18E-02CF810F91E8}"/>
     <hyperlink ref="H22" r:id="rId8" location="10402129" display="https://stackoverflow.com/questions/4181198/how-to-hash-a-password/10402129 - 10402129" xr:uid="{97C9D8AD-91DA-4ABA-B1F9-09B7B6B3C10F}"/>
+    <hyperlink ref="H23" r:id="rId9" xr:uid="{67312FB8-9D20-4747-98A4-8C6FEDD595A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1556,7 +1642,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0130828A-ACDD-452C-A113-199680C5AA6C}">
           <x14:formula1>
-            <xm:f>Données!$A$2:$A$9</xm:f>
+            <xm:f>Données!$A$2:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E31</xm:sqref>
         </x14:dataValidation>
@@ -1568,10 +1654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1708,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
@@ -1630,7 +1716,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1638,11 +1724,21 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Les contacts s'affichent et les messages peuvent être envoyés.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9781AB7C-93AD-43A8-845C-8FBA4C4F64F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792C4324-8DD4-4B1D-A500-B949A4EEB89D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>Les systèmes de création d'un compte et de login sont terminés. Mais pour l'instant, le mot de passe est stocké en clair car le hashage ne fonctionne pas.</t>
+  </si>
+  <si>
+    <t>22 mai</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Nous pouvons maintenant voir quel utilisateur est connecté.</t>
   </si>
 </sst>
 </file>
@@ -885,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,7 +1277,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D25" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D26" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1542,14 +1551,29 @@
       <c r="G25" s="27"/>
       <c r="H25" s="21"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="19"/>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>68</v>
+      </c>
       <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1642,7 +1666,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0130828A-ACDD-452C-A113-199680C5AA6C}">
           <x14:formula1>
-            <xm:f>Données!$A$2:$A$11</xm:f>
+            <xm:f>Données!$A$2:$A$12</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E31</xm:sqref>
         </x14:dataValidation>
@@ -1654,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,7 +1724,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1708,7 +1732,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
@@ -1716,7 +1740,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1724,21 +1748,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Journal de travail du 26 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792C4324-8DD4-4B1D-A500-B949A4EEB89D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B181F9-4F6E-4D9B-A41D-81D36D2A3EE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -237,13 +237,22 @@
     <t>Les systèmes de création d'un compte et de login sont terminés. Mais pour l'instant, le mot de passe est stocké en clair car le hashage ne fonctionne pas.</t>
   </si>
   <si>
-    <t>22 mai</t>
-  </si>
-  <si>
     <t>Chat</t>
   </si>
   <si>
     <t>Nous pouvons maintenant voir quel utilisateur est connecté.</t>
+  </si>
+  <si>
+    <t>22 mai 2020</t>
+  </si>
+  <si>
+    <t>26 mai 2020</t>
+  </si>
+  <si>
+    <t>J'ai corrigé les bugs lors de l'envoi des utilisateurs connectés et non connectés et j'ai avancé dans la réalisation du chat.</t>
+  </si>
+  <si>
+    <t>Les messages peuvent maintenant être envoyés, mais il reste des bugs d'affichage.</t>
   </si>
 </sst>
 </file>
@@ -894,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1286,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D26" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D28" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1553,7 +1562,7 @@
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B26" s="4">
         <v>0.33333333333333331</v>
@@ -1566,34 +1575,64 @@
         <v>0.16666666666666669</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="19"/>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="19"/>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1724,7 +1763,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Journal de travail du 27 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B181F9-4F6E-4D9B-A41D-81D36D2A3EE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB409523-9CAE-486D-AE6C-A041396FFB60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -253,6 +253,16 @@
   </si>
   <si>
     <t>Les messages peuvent maintenant être envoyés, mais il reste des bugs d'affichage.</t>
+  </si>
+  <si>
+    <t>27 mai 2020</t>
+  </si>
+  <si>
+    <t>Les messages sont affichés correctement mais il y a des problèmes avec la scrollbar.
+Je n'ai toujours pas réussi à actualiser les messages automatiquement (pour les recevoir en temps réel).</t>
+  </si>
+  <si>
+    <t>Les client peuvent maintenant se déconnecter.</t>
   </si>
 </sst>
 </file>
@@ -904,7 +914,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1296,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D28" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D30" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1635,24 +1645,54 @@
       </c>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="19"/>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="19"/>
+      <c r="A30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mise en forme du code et ajout des commentaires.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB409523-9CAE-486D-AE6C-A041396FFB60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FBA926-6FC1-4D5D-A562-16963048C9A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -263,6 +263,20 @@
   </si>
   <si>
     <t>Les client peuvent maintenant se déconnecter.</t>
+  </si>
+  <si>
+    <t>28 mai 2020</t>
+  </si>
+  <si>
+    <t>J'ai envoyé les executables au chef de projet.</t>
+  </si>
+  <si>
+    <t>L'affichage de tous les formulaires a été mis au propre.
+Les formulaires se ferment correctement maintenant.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/17752970/how-to-programmatically-scroll-a-panel
+https://stackoverflow.com/questions/13381127/preventing-winform-from-being-maximized</t>
   </si>
 </sst>
 </file>
@@ -523,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,7 +597,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -914,7 +927,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G39" sqref="G37:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1309,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D30" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D31" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1461,7 +1474,7 @@
       <c r="F21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="23" t="s">
         <v>56</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -1488,7 +1501,7 @@
       <c r="F22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="24" t="s">
         <v>59</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -1542,7 +1555,7 @@
       <c r="F24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="25" t="s">
         <v>65</v>
       </c>
       <c r="H24" s="21"/>
@@ -1567,10 +1580,10 @@
       <c r="F25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="21"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>68</v>
       </c>
@@ -1578,11 +1591,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C26" s="4">
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16666666666666669</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>66</v>
@@ -1590,49 +1603,47 @@
       <c r="F26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="19" t="s">
-        <v>67</v>
-      </c>
+      <c r="G26" s="10"/>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C27" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" ref="D27" ca="1" si="2">IF(ISBLANK(C27), NOW(),C27)-IF(ISBLANK(B27),NOW(),B27)</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="C28" s="4">
         <v>0.5</v>
       </c>
-      <c r="D27" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.16666666666666669</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="4">
-        <v>0.5625</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.60416666666666663</v>
-      </c>
       <c r="D28" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.166666666666663E-2</v>
+        <f t="shared" ref="D28" ca="1" si="3">IF(ISBLANK(C28), NOW(),C28)-IF(ISBLANK(B28),NOW(),B28)</f>
+        <v>6.25E-2</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>66</v>
@@ -1640,24 +1651,22 @@
       <c r="F28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="19" t="s">
-        <v>71</v>
-      </c>
+      <c r="G28" s="19"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B29" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="C29" s="4">
-        <v>0.5</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.16666666666666669</v>
+        <f t="shared" ref="D29" ca="1" si="4">IF(ISBLANK(C29), NOW(),C29)-IF(ISBLANK(B29),NOW(),B29)</f>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>66</v>
@@ -1666,49 +1675,138 @@
         <v>12</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B30" s="4">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C30" s="4">
-        <v>0.60416666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.166666666666663E-2</v>
+        <f ca="1">IF(ISBLANK(C30), NOW(),C30)-IF(ISBLANK(B30),NOW(),B30)</f>
+        <v>0.16666666666666669</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D31" s="4">
+        <f ca="1">IF(ISBLANK(C31), NOW(),C31)-IF(ISBLANK(B31),NOW(),B31)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="21"/>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="4">
+        <f ca="1">IF(ISBLANK(C32), NOW(),C32)-IF(ISBLANK(B32),NOW(),B32)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D33" s="4">
+        <f ca="1">IF(ISBLANK(C33), NOW(),C33)-IF(ISBLANK(B33),NOW(),B33)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H30" s="21"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="21"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="23"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="4">
+        <f ca="1">IF(ISBLANK(C34), NOW(),C34)-IF(ISBLANK(B34),NOW(),B34)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D35" s="22"/>
     </row>
   </sheetData>
@@ -1726,6 +1824,7 @@
     <hyperlink ref="H19" r:id="rId7" display="https://www.youtube.com/watch?v=Bq1JhTHlxek" xr:uid="{A1B3EF7B-1A3A-49EE-B18E-02CF810F91E8}"/>
     <hyperlink ref="H22" r:id="rId8" location="10402129" display="https://stackoverflow.com/questions/4181198/how-to-hash-a-password/10402129 - 10402129" xr:uid="{97C9D8AD-91DA-4ABA-B1F9-09B7B6B3C10F}"/>
     <hyperlink ref="H23" r:id="rId9" xr:uid="{67312FB8-9D20-4747-98A4-8C6FEDD595A0}"/>
+    <hyperlink ref="H34" r:id="rId10" display="https://stackoverflow.com/questions/17752970/how-to-programmatically-scroll-a-panel" xr:uid="{EFF0F916-1880-43D2-8936-44AFF558F17A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1735,7 +1834,7 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F31</xm:sqref>
+          <xm:sqref>F2:F15 F17:F34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
@@ -1747,7 +1846,7 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E31</xm:sqref>
+          <xm:sqref>E2:E34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Journal de travail du 28 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FBA926-6FC1-4D5D-A562-16963048C9A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A3A73E-3898-436F-A3AF-A9A01E26949F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -277,6 +277,9 @@
   <si>
     <t>https://stackoverflow.com/questions/17752970/how-to-programmatically-scroll-a-panel
 https://stackoverflow.com/questions/13381127/preventing-winform-from-being-maximized</t>
+  </si>
+  <si>
+    <t>Il ne peut maintenant y avoir qu'un utilisateur connecté par compte.</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,7 +599,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -927,7 +929,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G39" sqref="G37:G39"/>
+      <selection activeCell="E39" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1311,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15:D31" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
+        <f t="shared" ref="D15:D26" ca="1" si="1">IF(ISBLANK(C15), NOW(),C15)-IF(ISBLANK(B15),NOW(),B15)</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1474,7 +1476,7 @@
       <c r="F21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="22" t="s">
         <v>56</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -1501,7 +1503,7 @@
       <c r="F22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="23" t="s">
         <v>59</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -1555,7 +1557,7 @@
       <c r="F24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="24" t="s">
         <v>65</v>
       </c>
       <c r="H24" s="21"/>
@@ -1580,7 +1582,7 @@
       <c r="F25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="26"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,8 +1808,30 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="22"/>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D35" s="4">
+        <f ca="1">IF(ISBLANK(C35), NOW(),C35)-IF(ISBLANK(B35),NOW(),B35)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1834,7 +1858,7 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F34</xm:sqref>
+          <xm:sqref>F2:F15 F17:F35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
@@ -1846,7 +1870,7 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E34</xm:sqref>
+          <xm:sqref>E2:E35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Journal de travail du 29 mai.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A3A73E-3898-436F-A3AF-A9A01E26949F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20004314-1231-4DF0-8A11-A5617338C487}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -280,6 +280,16 @@
   </si>
   <si>
     <t>Il ne peut maintenant y avoir qu'un utilisateur connecté par compte.</t>
+  </si>
+  <si>
+    <t>29 mai 2020</t>
+  </si>
+  <si>
+    <t>Le programme est fonctionnel. Il reste la sécurisation des mots de passe et l'actualisation du chat.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/1450774/splitting-a-string-into-chunks-of-a-certain-size
+https://stackoverflow.com/questions/15564944/remove-the-last-three-characters-from-a-string/15564958</t>
   </si>
 </sst>
 </file>
@@ -344,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -535,12 +545,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -610,6 +685,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -926,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E39" sqref="E38:E39"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,7 +1782,7 @@
         <v>0.5</v>
       </c>
       <c r="D30" s="4">
-        <f ca="1">IF(ISBLANK(C30), NOW(),C30)-IF(ISBLANK(B30),NOW(),B30)</f>
+        <f t="shared" ref="D30:D35" ca="1" si="5">IF(ISBLANK(C30), NOW(),C30)-IF(ISBLANK(B30),NOW(),B30)</f>
         <v>0.16666666666666669</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -1717,7 +1807,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D31" s="4">
-        <f ca="1">IF(ISBLANK(C31), NOW(),C31)-IF(ISBLANK(B31),NOW(),B31)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -1742,7 +1832,7 @@
         <v>0.5</v>
       </c>
       <c r="D32" s="4">
-        <f ca="1">IF(ISBLANK(C32), NOW(),C32)-IF(ISBLANK(B32),NOW(),B32)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.16666666666666669</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -1767,7 +1857,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D33" s="4">
-        <f ca="1">IF(ISBLANK(C33), NOW(),C33)-IF(ISBLANK(B33),NOW(),B33)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -1792,7 +1882,7 @@
         <v>0.5</v>
       </c>
       <c r="D34" s="4">
-        <f ca="1">IF(ISBLANK(C34), NOW(),C34)-IF(ISBLANK(B34),NOW(),B34)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.16666666666666669</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -1819,7 +1909,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D35" s="4">
-        <f ca="1">IF(ISBLANK(C35), NOW(),C35)-IF(ISBLANK(B35),NOW(),B35)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -1833,9 +1923,59 @@
       </c>
       <c r="H35" s="21"/>
     </row>
+    <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" ref="D36" ca="1" si="6">IF(ISBLANK(C36), NOW(),C36)-IF(ISBLANK(B36),NOW(),B36)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" ref="D37" ca="1" si="7">IF(ISBLANK(C37), NOW(),C37)-IF(ISBLANK(B37),NOW(),B37)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="30"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="G24:G25"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1858,7 +1998,7 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F35</xm:sqref>
+          <xm:sqref>F2:F15 F17:F36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
@@ -1870,7 +2010,7 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E35</xm:sqref>
+          <xm:sqref>E2:E36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Travail du 2 juin.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20004314-1231-4DF0-8A11-A5617338C487}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB09EA3-C196-42EC-B184-5CBDF3569801}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activités" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -290,6 +290,23 @@
   <si>
     <t>https://stackoverflow.com/questions/1450774/splitting-a-string-into-chunks-of-a-certain-size
 https://stackoverflow.com/questions/15564944/remove-the-last-three-characters-from-a-string/15564958</t>
+  </si>
+  <si>
+    <t>2 juin 2020</t>
+  </si>
+  <si>
+    <t>J'ai fait quelques modifications sur l'affichage du chat et j'ai ajouté le système de hachage du mot de passe. L'application est maintenant terminée.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/4181198/how-to-hash-a-password</t>
+  </si>
+  <si>
+    <t>J'ai rédigé l'analyse concurentielle.
+J'ai rédigé les modification sur la partie graphique.</t>
+  </si>
+  <si>
+    <t>J'ai rédigé les icônes utilisées.
+J'ai rédigé les librairies utilisées.</t>
   </si>
 </sst>
 </file>
@@ -615,7 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -692,14 +709,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1016,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,10 +1963,10 @@
       <c r="F36" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="H36" s="29" t="s">
+      <c r="H36" s="28" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1961,13 +1981,90 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" ref="D37" ca="1" si="7">IF(ISBLANK(C37), NOW(),C37)-IF(ISBLANK(B37),NOW(),B37)</f>
+        <f t="shared" ref="D37:D38" ca="1" si="7">IF(ISBLANK(C37), NOW(),C37)-IF(ISBLANK(B37),NOW(),B37)</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="30"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="29"/>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" ca="1" si="7"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" ref="D39" ca="1" si="8">IF(ISBLANK(C39), NOW(),C39)-IF(ISBLANK(B39),NOW(),B39)</f>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" ref="D40" ca="1" si="9">IF(ISBLANK(C40), NOW(),C40)-IF(ISBLANK(B40),NOW(),B40)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1989,6 +2086,7 @@
     <hyperlink ref="H22" r:id="rId8" location="10402129" display="https://stackoverflow.com/questions/4181198/how-to-hash-a-password/10402129 - 10402129" xr:uid="{97C9D8AD-91DA-4ABA-B1F9-09B7B6B3C10F}"/>
     <hyperlink ref="H23" r:id="rId9" xr:uid="{67312FB8-9D20-4747-98A4-8C6FEDD595A0}"/>
     <hyperlink ref="H34" r:id="rId10" display="https://stackoverflow.com/questions/17752970/how-to-programmatically-scroll-a-panel" xr:uid="{EFF0F916-1880-43D2-8936-44AFF558F17A}"/>
+    <hyperlink ref="H38" r:id="rId11" xr:uid="{AF6BF814-3F07-4A39-B507-32648A7BE182}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1998,7 +2096,7 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F36</xm:sqref>
+          <xm:sqref>F2:F15 F17:F36 F38:F40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
@@ -2010,7 +2108,7 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E36</xm:sqref>
+          <xm:sqref>E2:E36 E38:E40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Journal de travail du 3 juin.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB09EA3-C196-42EC-B184-5CBDF3569801}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC7F76A-3D06-44A8-9454-0D79747B4D7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activités" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -307,6 +307,15 @@
   <si>
     <t>J'ai rédigé les icônes utilisées.
 J'ai rédigé les librairies utilisées.</t>
+  </si>
+  <si>
+    <t>3 juin 2020</t>
+  </si>
+  <si>
+    <t>J'ai rédigé la description des tests puis mon père et ma sœur ont testé mon application.</t>
+  </si>
+  <si>
+    <t>J'ai rédigé les erreurs restantes.</t>
   </si>
 </sst>
 </file>
@@ -709,17 +718,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1036,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,10 +1972,10 @@
       <c r="F36" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G36" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="30" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1986,8 +1995,8 @@
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="31"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2065,6 +2074,56 @@
         <v>87</v>
       </c>
       <c r="H40" s="21"/>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" ref="D41" ca="1" si="10">IF(ISBLANK(C41), NOW(),C41)-IF(ISBLANK(B41),NOW(),B41)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" s="21"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" ref="D42" ca="1" si="11">IF(ISBLANK(C42), NOW(),C42)-IF(ISBLANK(B42),NOW(),B42)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2096,7 +2155,7 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F36 F38:F40</xm:sqref>
+          <xm:sqref>F2:F15 F17:F36 F38:F42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
@@ -2108,7 +2167,7 @@
           <x14:formula1>
             <xm:f>Données!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E36 E38:E40</xm:sqref>
+          <xm:sqref>E2:E36 E38:E42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fin du projet et rendu final.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\MessagingApp\MessagingApp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC7F76A-3D06-44A8-9454-0D79747B4D7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1337F55F-A245-420F-9A03-2609B86B9A02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -316,6 +316,21 @@
   </si>
   <si>
     <t>J'ai rédigé les erreurs restantes.</t>
+  </si>
+  <si>
+    <t>4 juin 2020</t>
+  </si>
+  <si>
+    <t>J'ai terminé le rapport de projet.</t>
+  </si>
+  <si>
+    <t>5 juin 2020</t>
+  </si>
+  <si>
+    <t>Manuel d'utilisation</t>
+  </si>
+  <si>
+    <t>J'ai rédigé un manuel d'utilisation</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45:G46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G41" s="19" t="s">
         <v>89</v>
@@ -2111,7 +2126,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" ref="D42" ca="1" si="11">IF(ISBLANK(C42), NOW(),C42)-IF(ISBLANK(B42),NOW(),B42)</f>
+        <f t="shared" ref="D42:D43" ca="1" si="11">IF(ISBLANK(C42), NOW(),C42)-IF(ISBLANK(B42),NOW(),B42)</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -2125,8 +2140,81 @@
       </c>
       <c r="H42" s="21"/>
     </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" ca="1" si="11"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="H43" s="30"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" ref="D44:D45" ca="1" si="12">IF(ISBLANK(C44), NOW(),C44)-IF(ISBLANK(B44),NOW(),B44)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="31"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" s="21"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="F36:F37"/>
@@ -2155,19 +2243,19 @@
           <x14:formula1>
             <xm:f>Données!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15 F17:F36 F38:F42</xm:sqref>
+          <xm:sqref>F2:F15 F17:F36 F45 F38:F40 F42:F43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220D63A3-DD64-46A4-890C-79BF9F0ACDAE}">
           <x14:formula1>
             <xm:f>Données!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F16</xm:sqref>
+          <xm:sqref>F16 F41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0130828A-ACDD-452C-A113-199680C5AA6C}">
           <x14:formula1>
-            <xm:f>Données!$A$2:$A$12</xm:f>
+            <xm:f>Données!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E36 E38:E42</xm:sqref>
+          <xm:sqref>E2:E36 E45 E38:E43</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2177,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,21 +2340,26 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>